<commit_message>
Added learn GitHub task
learn GitHub task
</commit_message>
<xml_diff>
--- a/JADD_story_board_v001.xlsx
+++ b/JADD_story_board_v001.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Project Proposal</t>
   </si>
@@ -290,6 +290,12 @@
   </si>
   <si>
     <t>Kermit the Frog</t>
+  </si>
+  <si>
+    <t>Understand how to upload code in iterations on GitHub</t>
+  </si>
+  <si>
+    <t>Dan</t>
   </si>
 </sst>
 </file>
@@ -921,14 +927,13 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.33203125" customWidth="1"/>
-    <col min="2" max="2" width="38.33203125" customWidth="1"/>
-    <col min="3" max="3" width="21.33203125" customWidth="1"/>
+    <col min="2" max="3" width="43.6640625" customWidth="1"/>
     <col min="4" max="4" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -994,6 +999,12 @@
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" t="s">
+        <v>43</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>